<commit_message>
added alphapose and qol
added alphapose and other qol improvements.
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -22,22 +22,22 @@
     <t>typ filmu</t>
   </si>
   <si>
+    <t>Brakujące klatki</t>
+  </si>
+  <si>
+    <t>Poprawność klasyfikatora</t>
+  </si>
+  <si>
     <t>ilość punktów</t>
   </si>
   <si>
-    <t>Poprawność klasyfikatora</t>
-  </si>
-  <si>
-    <t>wynik</t>
-  </si>
-  <si>
-    <t>Openpose</t>
-  </si>
-  <si>
-    <t>Blazepose</t>
-  </si>
-  <si>
-    <t>Deeppose</t>
+    <t>BlazePose</t>
+  </si>
+  <si>
+    <t>OpenPose</t>
+  </si>
+  <si>
+    <t>AlphaPose</t>
   </si>
   <si>
     <t>f1 norma</t>
@@ -49,6 +49,9 @@
     <t>f1 zakrycie</t>
   </si>
   <si>
+    <t>f1 oba</t>
+  </si>
+  <si>
     <t>f2 norma</t>
   </si>
   <si>
@@ -56,6 +59,9 @@
   </si>
   <si>
     <t>f2 zakrycie</t>
+  </si>
+  <si>
+    <t>f2 oba</t>
   </si>
 </sst>
 </file>
@@ -413,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -444,13 +450,10 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>32896</v>
+        <v>9</v>
       </c>
       <c r="D2">
-        <v>0.9893924783027965</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
+        <v>0.8910318225650916</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -458,13 +461,10 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
+        <v>0.6730954676952748</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -472,13 +472,10 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>244</v>
       </c>
       <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
+        <v>0.5332690453230472</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -486,13 +483,10 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>367</v>
       </c>
       <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
+        <v>0.4503375120540019</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -500,13 +494,10 @@
         <v>12</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
+        <v>0.7129543336439889</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -514,187 +505,214 @@
         <v>13</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
+        <v>0.5983224603914259</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C8">
-        <v>25600</v>
+        <v>131</v>
       </c>
       <c r="D8">
-        <v>0.9074252651880425</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
+        <v>0.6132339235787512</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="B9" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>298</v>
       </c>
       <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
+        <v>0.5955265610438024</v>
       </c>
     </row>
     <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
+        <v>0.8119575699132112</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="B11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
+        <v>0.5805207328833173</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="B12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
+        <v>0.5940212150433944</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="B13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
+        <v>0.5332690453230472</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
+        <v>0.7502329916123019</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="B15" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
+        <v>0.5517241379310345</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>0.527493010251631</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>90</v>
+      </c>
+      <c r="D17">
+        <v>0.5405405405405406</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>298</v>
+      </c>
+      <c r="D18">
+        <v>0.8871745419479267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0.5226615236258437</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="B20" t="s">
         <v>10</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" t="s">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0.3278688524590164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="B21" t="s">
         <v>11</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" t="s">
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0.5429122468659595</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="B22" t="s">
         <v>12</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" t="s">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0.6728797763280522</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="B23" t="s">
         <v>13</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0.4986020503261883</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0.4986020503261883</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>0.4958061509785648</v>
       </c>
     </row>
   </sheetData>

</xml_diff>